<commit_message>
Bug fixes Random employee number Export data only at successful action Excel updated
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>JavaDoc</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>לתקן את השמירה רק לכל פעולה מוצלחת</t>
+  </si>
+  <si>
+    <t>מספר עובד רנדומלי</t>
   </si>
 </sst>
 </file>
@@ -60,12 +63,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -80,11 +89,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -399,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B8"/>
+  <dimension ref="B2:B9"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,11 +451,17 @@
       </c>
     </row>
     <row r="8" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed all the shit you've done I took care of something like 10 null Exceptions because you did nothing to take care of null DB
</commit_message>
<xml_diff>
--- a/Tasks.xlsx
+++ b/Tasks.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nisan\Documents\newIShape\virutalshape5\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micke\Documents\NetBeansProjects\virutalshape\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>JavaDoc</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>מספר עובד רנדומלי</t>
+  </si>
+  <si>
+    <t>כאשר המערכת ריקה ולוחצים על שאילתה מקבלים Exception</t>
+  </si>
+  <si>
+    <t>להוסיף יוזר ADMIN שלא נמצא על DB וניתן לעלות איתו תמיד</t>
   </si>
 </sst>
 </file>
@@ -426,55 +432,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:B9"/>
+  <dimension ref="B2:B11"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="65.44140625" customWidth="1"/>
+    <col min="2" max="2" width="65.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>